<commit_message>
i add add  my picture and  name to the team section
</commit_message>
<xml_diff>
--- a/Task.xlsx
+++ b/Task.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>name</t>
   </si>
@@ -117,7 +117,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -125,14 +125,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -462,7 +462,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -497,7 +497,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -708,19 +708,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="23.25" style="1" customWidth="1"/>
     <col min="2" max="2" width="57" style="3" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="18.25" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="20.25" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -731,7 +731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
@@ -740,7 +740,7 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
@@ -751,7 +751,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
@@ -760,7 +760,7 @@
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>6</v>
       </c>
@@ -769,7 +769,7 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
@@ -778,16 +778,18 @@
       </c>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C7" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>12</v>
       </c>
@@ -796,7 +798,7 @@
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
         <v>9</v>
       </c>
@@ -805,7 +807,7 @@
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>10</v>
       </c>
@@ -814,7 +816,7 @@
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
         <v>11</v>
       </c>
@@ -823,7 +825,7 @@
       </c>
       <c r="C11" s="4"/>
     </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>13</v>
       </c>
@@ -832,7 +834,7 @@
       </c>
       <c r="C12" s="4"/>
     </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>14</v>
       </c>
@@ -841,7 +843,7 @@
       </c>
       <c r="C13" s="4"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>15</v>
       </c>
@@ -852,7 +854,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>16</v>
       </c>
@@ -861,7 +863,7 @@
       </c>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>17</v>
       </c>

</xml_diff>